<commit_message>
updates to model files
</commit_message>
<xml_diff>
--- a/Interpolat_Diff_Tax/Money_Analysis/US_China_Group_Price.xlsx
+++ b/Interpolat_Diff_Tax/Money_Analysis/US_China_Group_Price.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorgan/Documents/PostDoc/Diff_Tax_Analysis/Theoretical_Analysis/Interpolat_Diff_Tax/Money_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1781835-DEE0-ED47-86DD-68C93A21224C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64E8C27-C593-A749-98C0-588845A60B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="4960" windowWidth="18780" windowHeight="14940" xr2:uid="{57EAA5CF-5E39-1A4F-9399-76395567C3D1}"/>
+    <workbookView xWindow="25180" yWindow="5080" windowWidth="18780" windowHeight="14940" xr2:uid="{57EAA5CF-5E39-1A4F-9399-76395567C3D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,10 +531,10 @@
         <v>292.47699999999998</v>
       </c>
       <c r="L2">
-        <v>2165.4366437967465</v>
+        <v>980.58</v>
       </c>
       <c r="M2">
-        <v>7041.5705965716988</v>
+        <v>5984.73</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -610,7 +610,7 @@
         <v>3</v>
       </c>
       <c r="K4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -651,7 +651,7 @@
         <v>2</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -771,7 +771,7 @@
         <v>29919416530.15873</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f>H2*H6</f>
         <v>8685287999.9999981</v>
       </c>
       <c r="I8">
@@ -788,11 +788,11 @@
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>372455102.73304039</v>
+        <v>168659760</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>3485577445.3029909</v>
+        <v>2962441350</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>